<commit_message>
Updated metadata after matching with vebanny generation code
</commit_message>
<xml_diff>
--- a/docs/veBanny-layered-assets/banny-names-metadata-histories-mottos.xlsx
+++ b/docs/veBanny-layered-assets/banny-names-metadata-histories-mottos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mark.phillips/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mark.phillips/Developer/bannyverse-app/docs/veBanny-layered-assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{811AA063-3BA5-E946-9E1D-0E9D3FB365C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F30D5D-02B2-CB44-8C1B-45934AE461D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-57080" yWindow="-5000" windowWidth="52160" windowHeight="31720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1244,7 +1244,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:XFD1048576"/>
+      <selection activeCell="C2" sqref="C2:C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>